<commit_message>
Aggiornati files per accreditamenti
Aggiornati files per accreditamenti:
* AffideaHCIS-AMB
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#AFFIDEAXX/AFFIDEA/AffideaHCIS-AMB/V.12.0/accreditamento-checklist_V8.2.6-AMB.xlsx
+++ b/GATEWAY/A1#111#AFFIDEAXX/AFFIDEA/AffideaHCIS-AMB/V.12.0/accreditamento-checklist_V8.2.6-AMB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ombretta.bonino\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test\accreditamento-sogei\CDA2-AMB\CASE_TEST_invio_2025-07-07\A1#111#AFFIDEAXX\AffideaHCIS-AMB\V.12.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF42E44-831D-4577-99B7-BB8A5BA8C566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062B4384-44BE-4ECE-9B8E-9DB7308C7CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5400" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1900,24 +1900,6 @@
     <t>13:22:08.664</t>
   </si>
   <si>
-    <t>51479e916c16d1a6ef07f385e55f8683</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4.4.f845a952550a3048fc725df3036c3a79b9621f252b86ea1da115ff63db3eb8f3.ec0e8eed9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>12:54:31.594</t>
-  </si>
-  <si>
-    <t>2635968315cba9c730ba9f194505f65a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4.4.344fbf14f3ff6947812503a249cf927119609344ac9b299212dc569e235debb9.48b21f5701^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>12:57:04.033</t>
-  </si>
-  <si>
     <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-44| Il codice fiscale 'nnmnnm56r28l219a' cittadino ed operatore deve essere costituito da 16 cifre [A-Z0-9]{16}]</t>
   </si>
   <si>
@@ -1986,6 +1968,24 @@
   </si>
   <si>
     <t>Validazione FSE Gateway: [Timeout o annullamento] L'operazione è stata annullata o ha impiegato troppo tempo. The request was canceled due to the configured HttpClient.Timeout of 0,001 seconds elapsing.</t>
+  </si>
+  <si>
+    <t>1a60cf16dbc7377123386c30a83ba48f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.f845a952550a3048fc725df3036c3a79b9621f252b86ea1da115ff63db3eb8f3.ba310e5968^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>11:56:38.533</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.344fbf14f3ff6947812503a249cf927119609344ac9b299212dc569e235debb9.56b4ce2872^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d01ade9110368f9c7de3f395c4c69e3d</t>
+  </si>
+  <si>
+    <t>12:00:23.290</t>
   </si>
 </sst>
 </file>
@@ -4158,10 +4158,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="14" topLeftCell="M15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="14" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="O31" sqref="O31"/>
+      <selection pane="bottomRight" activeCell="H200" sqref="H200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4674,7 +4674,7 @@
         <v>64</v>
       </c>
       <c r="O15" s="60" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="P15" s="38" t="s">
         <v>64</v>
@@ -4994,7 +4994,7 @@
         <v>64</v>
       </c>
       <c r="O23" s="60" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="P23" s="38" t="s">
         <v>64</v>
@@ -5314,7 +5314,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="60" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="P31" s="38" t="s">
         <v>64</v>
@@ -8491,7 +8491,7 @@
         <v>64</v>
       </c>
       <c r="O116" s="60" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="P116" s="38" t="s">
         <v>64</v>
@@ -8552,7 +8552,7 @@
         <v>64</v>
       </c>
       <c r="O117" s="60" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="P117" s="38" t="s">
         <v>64</v>
@@ -8613,7 +8613,7 @@
         <v>64</v>
       </c>
       <c r="O118" s="60" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="P118" s="38" t="s">
         <v>64</v>
@@ -8674,7 +8674,7 @@
         <v>64</v>
       </c>
       <c r="O119" s="60" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="P119" s="38" t="s">
         <v>64</v>
@@ -8735,7 +8735,7 @@
         <v>64</v>
       </c>
       <c r="O120" s="60" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="P120" s="38" t="s">
         <v>64</v>
@@ -8796,7 +8796,7 @@
         <v>64</v>
       </c>
       <c r="O121" s="60" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="P121" s="38" t="s">
         <v>64</v>
@@ -8857,7 +8857,7 @@
         <v>64</v>
       </c>
       <c r="O122" s="60" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="P122" s="38" t="s">
         <v>64</v>
@@ -8918,7 +8918,7 @@
         <v>64</v>
       </c>
       <c r="O123" s="60" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="P123" s="38" t="s">
         <v>64</v>
@@ -8979,7 +8979,7 @@
         <v>64</v>
       </c>
       <c r="O124" s="60" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="P124" s="38" t="s">
         <v>64</v>
@@ -9020,13 +9020,13 @@
         <v>45833</v>
       </c>
       <c r="G125" s="65" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="H125" s="66" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="I125" s="67" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="J125" s="68" t="s">
         <v>64</v>
@@ -9040,7 +9040,7 @@
         <v>64</v>
       </c>
       <c r="O125" s="69" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="P125" s="68" t="s">
         <v>64</v>
@@ -9101,7 +9101,7 @@
         <v>64</v>
       </c>
       <c r="O126" s="60" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="P126" s="38" t="s">
         <v>64</v>
@@ -9162,7 +9162,7 @@
         <v>64</v>
       </c>
       <c r="O127" s="60" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="P127" s="38" t="s">
         <v>64</v>
@@ -9223,7 +9223,7 @@
         <v>64</v>
       </c>
       <c r="O128" s="60" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="P128" s="38" t="s">
         <v>64</v>
@@ -9284,7 +9284,7 @@
         <v>64</v>
       </c>
       <c r="O129" s="60" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="P129" s="38" t="s">
         <v>64</v>
@@ -9345,7 +9345,7 @@
         <v>64</v>
       </c>
       <c r="O130" s="60" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="P130" s="38" t="s">
         <v>64</v>
@@ -10678,16 +10678,16 @@
         <v>389</v>
       </c>
       <c r="F166" s="48">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="G166" s="48" t="s">
-        <v>500</v>
+        <v>523</v>
       </c>
       <c r="H166" s="56" t="s">
-        <v>498</v>
+        <v>521</v>
       </c>
       <c r="I166" s="57" t="s">
-        <v>499</v>
+        <v>522</v>
       </c>
       <c r="J166" s="49" t="s">
         <v>64</v>
@@ -10725,16 +10725,16 @@
         <v>390</v>
       </c>
       <c r="F167" s="48">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="G167" s="48" t="s">
-        <v>503</v>
+        <v>526</v>
       </c>
       <c r="H167" s="56" t="s">
-        <v>501</v>
+        <v>525</v>
       </c>
       <c r="I167" s="57" t="s">
-        <v>502</v>
+        <v>524</v>
       </c>
       <c r="J167" s="49" t="s">
         <v>64</v>
@@ -11165,7 +11165,7 @@
         <v>64</v>
       </c>
       <c r="O178" s="60" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="P178" s="38" t="s">
         <v>64</v>
@@ -11448,7 +11448,7 @@
         <v>64</v>
       </c>
       <c r="O185" s="60" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="P185" s="38" t="s">
         <v>64</v>
@@ -11731,7 +11731,7 @@
         <v>64</v>
       </c>
       <c r="O192" s="60" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="P192" s="38" t="s">
         <v>64</v>
@@ -18071,27 +18071,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -18349,32 +18328,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18393,6 +18368,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>